<commit_message>
Agrega última información de los piers
</commit_message>
<xml_diff>
--- a/Tarea 03/muros.xlsx
+++ b/Tarea 03/muros.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{376D4F42-6667-4D8F-B529-218ED8A7B2A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PIERS" sheetId="1" r:id="rId1"/>
+    <sheet name="EJE Y" sheetId="2" r:id="rId2"/>
+    <sheet name="EJE X" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,10 +21,83 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+  <si>
+    <t>Ejes</t>
+  </si>
+  <si>
+    <t>N° pier</t>
+  </si>
+  <si>
+    <t>A entre 1-2</t>
+  </si>
+  <si>
+    <t>M1Y</t>
+  </si>
+  <si>
+    <t>Largo (cm)</t>
+  </si>
+  <si>
+    <t>A entre 2-3</t>
+  </si>
+  <si>
+    <t>A entre 3-4</t>
+  </si>
+  <si>
+    <t>B entre 1-2</t>
+  </si>
+  <si>
+    <t>B entre 3-4</t>
+  </si>
+  <si>
+    <t>C entre 1-2</t>
+  </si>
+  <si>
+    <t>C entre 2-3</t>
+  </si>
+  <si>
+    <t>C entre 3-4</t>
+  </si>
+  <si>
+    <t>M2Y</t>
+  </si>
+  <si>
+    <t>M3Y</t>
+  </si>
+  <si>
+    <t>M4Y</t>
+  </si>
+  <si>
+    <t>M5Y</t>
+  </si>
+  <si>
+    <t>M6Y</t>
+  </si>
+  <si>
+    <t>M7Y</t>
+  </si>
+  <si>
+    <t>M8Y</t>
+  </si>
+  <si>
+    <t>Alto (cm)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +121,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +423,671 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51A635C-89FC-44BE-82EF-59DE5B63DCE1}">
+  <dimension ref="B2:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>390</v>
+      </c>
+      <c r="E3" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>225</v>
+      </c>
+      <c r="E4" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>390</v>
+      </c>
+      <c r="E5" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>390</v>
+      </c>
+      <c r="E6" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>390</v>
+      </c>
+      <c r="E7" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>390</v>
+      </c>
+      <c r="E8" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2">
+        <v>225</v>
+      </c>
+      <c r="E9" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2">
+        <v>390</v>
+      </c>
+      <c r="E10" s="2">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35158A57-6756-49F2-BC24-2FD64A7749BD}">
+  <dimension ref="A2:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>"M"&amp;A3&amp;"X"</f>
+        <v>M1X</v>
+      </c>
+      <c r="D3" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <f>A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f t="shared" ref="C4:C45" si="0">"M"&amp;A4&amp;"X"</f>
+        <v>M2X</v>
+      </c>
+      <c r="D4" s="2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <f t="shared" ref="A5:A50" si="1">A4+1</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M3X</v>
+      </c>
+      <c r="D5" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M4X</v>
+      </c>
+      <c r="D6" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M5X</v>
+      </c>
+      <c r="D7" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M6X</v>
+      </c>
+      <c r="D8" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M7X</v>
+      </c>
+      <c r="D9" s="2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M8X</v>
+      </c>
+      <c r="D10" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M9X</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M10X</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M11X</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M12X</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M13X</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M14X</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M15X</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M16X</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M17X</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M18X</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M19X</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M20X</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M21X</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M22X</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M23X</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M24X</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M25X</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M26X</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M27X</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M28X</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M29X</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M30X</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M31X</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M32X</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M33X</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M34X</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M35X</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M36X</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M37X</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M38X</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M39X</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M40X</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M41X</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M42X</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="C45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>M43X</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agrega concepto de geometrías
</commit_message>
<xml_diff>
--- a/Tarea 03/muros.xlsx
+++ b/Tarea 03/muros.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C1F85826-9FEF-443E-A2DC-CD896B1AA116}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B0F4BAEA-BF49-4220-837B-945F7306AEEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIERS" sheetId="1" r:id="rId1"/>
     <sheet name="EJE Y" sheetId="2" r:id="rId2"/>
     <sheet name="EJE X" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Ejes</t>
   </si>
@@ -103,12 +104,72 @@
   </si>
   <si>
     <t>4 entre B y C</t>
+  </si>
+  <si>
+    <t>Geometría</t>
+  </si>
+  <si>
+    <t>$\phi$</t>
+  </si>
+  <si>
+    <t>Piers</t>
+  </si>
+  <si>
+    <t>M1Y, M3Y, M4Y, M5, M6Y, M8Y</t>
+  </si>
+  <si>
+    <t>M2Y, M7Y</t>
+  </si>
+  <si>
+    <t>M1X, M13X</t>
+  </si>
+  <si>
+    <t>M2X, M14X</t>
+  </si>
+  <si>
+    <t>M3X, M6X, M15X</t>
+  </si>
+  <si>
+    <t>M4X, M16X</t>
+  </si>
+  <si>
+    <t>M5X</t>
+  </si>
+  <si>
+    <t>M7X</t>
+  </si>
+  <si>
+    <t>M8X, M21X</t>
+  </si>
+  <si>
+    <t>M9X</t>
+  </si>
+  <si>
+    <t>M10X % M10X, M12X</t>
+  </si>
+  <si>
+    <t>M11X</t>
+  </si>
+  <si>
+    <t>M12X</t>
+  </si>
+  <si>
+    <t>M13X</t>
+  </si>
+  <si>
+    <t>M14X</t>
+  </si>
+  <si>
+    <t>M15X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -153,16 +214,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -459,10 +553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51A635C-89FC-44BE-82EF-59DE5B63DCE1}">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,10 +565,11 @@
     <col min="2" max="2" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="2"/>
+    <col min="6" max="6" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -487,117 +582,172 @@
       <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>390</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="F3" s="4">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>225</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="F4" s="4">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>390</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="F5" s="4">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>390</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="F6" s="4">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>390</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="F7" s="4">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>390</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="F8" s="4">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>225</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="4">
         <v>260</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="F9" s="4">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>390</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>260</v>
+      </c>
+      <c r="F10" s="5">
+        <v>12</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -609,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35158A57-6756-49F2-BC24-2FD64A7749BD}">
   <dimension ref="B2:XFD23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,10 +770,11 @@
     <col min="3" max="3" width="11.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="2"/>
+    <col min="6" max="6" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -636,10 +787,16 @@
       <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="str">
-        <f>"M"&amp;XFD3&amp;"X"</f>
+        <f t="shared" ref="B3:B23" si="0">"M"&amp;XFD3&amp;"X"</f>
         <v>M1X</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -651,51 +808,69 @@
       <c r="E3" s="2">
         <v>94.6</v>
       </c>
+      <c r="F3" s="2">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
       <c r="XFD3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="str">
-        <f>"M"&amp;XFD4&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M2X</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="2">
-        <v>112.25</v>
+        <v>112</v>
       </c>
       <c r="E4" s="2">
         <v>113.4</v>
       </c>
+      <c r="F4" s="2">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
       <c r="XFD4" s="2">
-        <f>XFD3+1</f>
+        <f t="shared" ref="XFD4:XFD23" si="1">XFD3+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="str">
-        <f>"M"&amp;XFD5&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M3X</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>97.75</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2">
         <v>113.4</v>
       </c>
+      <c r="F5" s="2">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
       <c r="XFD5" s="2">
-        <f>XFD4+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
-        <f>"M"&amp;XFD6&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M4X</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -707,14 +882,20 @@
       <c r="E6" s="2">
         <v>52</v>
       </c>
+      <c r="F6" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6</v>
+      </c>
       <c r="XFD6" s="2">
-        <f>XFD5+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
-        <f>"M"&amp;XFD7&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M5X</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -726,52 +907,70 @@
       <c r="E7" s="2">
         <v>94.6</v>
       </c>
+      <c r="F7" s="2">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2">
+        <v>7</v>
+      </c>
       <c r="XFD7" s="2">
-        <f>XFD6+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
-        <f>"M"&amp;XFD8&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M6X</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="2">
-        <v>97.5</v>
+        <v>98</v>
       </c>
       <c r="E8" s="2">
         <v>113.4</v>
       </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
       <c r="XFD8" s="2">
-        <f>XFD7+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
-        <f>"M"&amp;XFD9&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M7X</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2">
-        <v>164.5</v>
+        <v>164</v>
       </c>
       <c r="E9" s="2">
         <v>113.4</v>
       </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
       <c r="XFD9" s="2">
-        <f>XFD8+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
-        <f>"M"&amp;XFD10&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M8X</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -783,14 +982,20 @@
       <c r="E10" s="2">
         <v>52</v>
       </c>
+      <c r="F10" s="2">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2">
+        <v>9</v>
+      </c>
       <c r="XFD10" s="2">
-        <f>XFD9+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
-        <f>"M"&amp;XFD11&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M9X</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -803,14 +1008,20 @@
         <f>113.4+94.6</f>
         <v>208</v>
       </c>
+      <c r="F11" s="2">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
       <c r="XFD11" s="2">
-        <f>XFD10+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="str">
-        <f>"M"&amp;XFD12&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M10X</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -822,14 +1033,20 @@
       <c r="E12" s="2">
         <v>260</v>
       </c>
+      <c r="F12" s="2">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2">
+        <v>11</v>
+      </c>
       <c r="XFD12" s="2">
-        <f>XFD11+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="str">
-        <f>"M"&amp;XFD13&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M11X</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -841,14 +1058,20 @@
       <c r="E13" s="2">
         <v>260</v>
       </c>
+      <c r="F13" s="2">
+        <v>12</v>
+      </c>
+      <c r="G13" s="2">
+        <v>12</v>
+      </c>
       <c r="XFD13" s="2">
-        <f>XFD12+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="str">
-        <f>"M"&amp;XFD14&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M12X</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -860,14 +1083,20 @@
       <c r="E14" s="2">
         <v>260</v>
       </c>
+      <c r="F14" s="2">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2">
+        <v>13</v>
+      </c>
       <c r="XFD14" s="2">
-        <f>XFD13+1</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="str">
-        <f>"M"&amp;XFD15&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M13X</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -879,14 +1108,20 @@
       <c r="E15" s="2">
         <v>94.6</v>
       </c>
+      <c r="F15" s="2">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3</v>
+      </c>
       <c r="XFD15" s="2">
-        <f>XFD14+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="str">
-        <f>"M"&amp;XFD16&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M14X</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -898,14 +1133,20 @@
       <c r="E16" s="2">
         <v>113.4</v>
       </c>
+      <c r="F16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4</v>
+      </c>
       <c r="XFD16" s="2">
-        <f>XFD15+1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
-        <f>"M"&amp;XFD17&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M15X</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -917,14 +1158,20 @@
       <c r="E17" s="2">
         <v>113.4</v>
       </c>
+      <c r="F17" s="2">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5</v>
+      </c>
       <c r="XFD17" s="2">
-        <f>XFD16+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="str">
-        <f>"M"&amp;XFD18&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M16X</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -936,14 +1183,20 @@
       <c r="E18" s="2">
         <v>52</v>
       </c>
+      <c r="F18" s="2">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
       <c r="XFD18" s="2">
-        <f>XFD17+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="str">
-        <f>"M"&amp;XFD19&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M17X</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -956,14 +1209,20 @@
         <f>113.4+94.6</f>
         <v>208</v>
       </c>
+      <c r="F19" s="2">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2">
+        <v>14</v>
+      </c>
       <c r="XFD19" s="2">
-        <f>XFD18+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="str">
-        <f>"M"&amp;XFD20&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M18X</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -975,14 +1234,20 @@
       <c r="E20" s="2">
         <v>94.6</v>
       </c>
+      <c r="F20" s="2">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2">
+        <v>15</v>
+      </c>
       <c r="XFD20" s="2">
-        <f>XFD19+1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="str">
-        <f>"M"&amp;XFD21&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M19X</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -994,14 +1259,20 @@
       <c r="E21" s="2">
         <v>113.4</v>
       </c>
+      <c r="F21" s="2">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2">
+        <v>8</v>
+      </c>
       <c r="XFD21" s="2">
-        <f>XFD20+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="str">
-        <f>"M"&amp;XFD22&amp;"X"</f>
+        <f t="shared" si="0"/>
         <v>M20X</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1013,31 +1284,201 @@
       <c r="E22" s="2">
         <v>113.4</v>
       </c>
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2">
+        <v>16</v>
+      </c>
       <c r="XFD22" s="2">
-        <f>XFD21+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="str">
-        <f>"M"&amp;XFD23&amp;"X"</f>
+    <row r="23" spans="2:7 16384:16384" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="str">
+        <f t="shared" si="0"/>
         <v>M21X</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="5">
         <v>510</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="5">
         <v>52</v>
       </c>
+      <c r="F23" s="5">
+        <v>12</v>
+      </c>
+      <c r="G23" s="5">
+        <v>9</v>
+      </c>
       <c r="XFD23" s="2">
-        <f>XFD22+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43D1540-3C5B-4A3C-993F-E678E3EE0B79}">
+  <dimension ref="B2:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="2"/>
+    <col min="3" max="3" width="26.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="7">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>